<commit_message>
Refactory: Correção na ortografia.
</commit_message>
<xml_diff>
--- a/Teste de Programação.xlsx
+++ b/Teste de Programação.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSVeras\Documents\source\repos\Nasa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSVeras\Documents\source\repos\Explorando-Marte\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1562,7 +1562,7 @@
       <c r="Q47" s="3"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="H48" s="2" t="s">
+      <c r="A48" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>